<commit_message>
Refactored solution to fit Coursera infrastructure
refactored the solution and added files to fit the coursera
infrastructure to allow test of solution and submission using coursera
scripts
</commit_message>
<xml_diff>
--- a/Week 1/Lecture Notes/KnapsackExample.xlsx
+++ b/Week 1/Lecture Notes/KnapsackExample.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="760" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ks_4_0" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>Maximise</t>
   </si>
@@ -115,6 +116,21 @@
   </si>
   <si>
     <t>finish</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>8x1 + 10x2 + 15x3 + 4x4</t>
+  </si>
+  <si>
+    <t>4x1 + 5x2 + 8x3 + 3x4 &lt;= 11</t>
+  </si>
+  <si>
+    <t>number of items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x4 + x3 </t>
   </si>
 </sst>
 </file>
@@ -393,8 +409,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -419,11 +437,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -755,7 +775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -1114,4 +1134,414 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16" thickBot="1"/>
+    <row r="10" spans="1:7" ht="16" thickBot="1">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4">
+        <v>10</v>
+      </c>
+      <c r="D12" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4">
+        <v>15</v>
+      </c>
+      <c r="D13" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16" thickBot="1">
+      <c r="B14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="7">
+        <v>4</v>
+      </c>
+      <c r="D14" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16" thickBot="1"/>
+    <row r="19" spans="1:7" ht="16" thickBot="1">
+      <c r="B19" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0</v>
+      </c>
+      <c r="D19" s="11">
+        <v>1</v>
+      </c>
+      <c r="E19" s="11">
+        <v>2</v>
+      </c>
+      <c r="F19" s="11">
+        <v>3</v>
+      </c>
+      <c r="G19" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="B20" s="13">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="B21" s="14">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="B22" s="14">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="B23" s="13">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="B24" s="14">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>8</v>
+      </c>
+      <c r="E24" s="2">
+        <v>8</v>
+      </c>
+      <c r="F24" s="2">
+        <v>8</v>
+      </c>
+      <c r="G24" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="B25" s="14">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2">
+        <v>10</v>
+      </c>
+      <c r="F25" s="2">
+        <v>10</v>
+      </c>
+      <c r="G25" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26" s="13">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>8</v>
+      </c>
+      <c r="E26" s="2">
+        <v>10</v>
+      </c>
+      <c r="F26" s="2">
+        <v>10</v>
+      </c>
+      <c r="G26" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="B27" s="14">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>8</v>
+      </c>
+      <c r="E27" s="2">
+        <v>10</v>
+      </c>
+      <c r="F27" s="2">
+        <v>10</v>
+      </c>
+      <c r="G27" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="B28" s="14">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
+        <v>8</v>
+      </c>
+      <c r="E28" s="2">
+        <v>10</v>
+      </c>
+      <c r="F28" s="2">
+        <v>15</v>
+      </c>
+      <c r="G28" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="B29" s="13">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" s="4">
+        <v>8</v>
+      </c>
+      <c r="E29" s="2">
+        <v>18</v>
+      </c>
+      <c r="F29" s="2">
+        <v>18</v>
+      </c>
+      <c r="G29" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="B30" s="14">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" s="4">
+        <v>8</v>
+      </c>
+      <c r="E30" s="2">
+        <v>18</v>
+      </c>
+      <c r="F30" s="2">
+        <v>18</v>
+      </c>
+      <c r="G30" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="B31" s="14">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4">
+        <v>8</v>
+      </c>
+      <c r="E31" s="2">
+        <v>18</v>
+      </c>
+      <c r="F31" s="2">
+        <v>18</v>
+      </c>
+      <c r="G31" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Submitted assignments - all but 4 & 6 successful
submitted all assignments after increasing heap size to maximum for
machine - all successful apart from 4 and 6 which failed due to heap
size.  Now need to implement branch and bound algorithm to try and
solve them
</commit_message>
<xml_diff>
--- a/Week 1/Lecture Notes/KnapsackExample.xlsx
+++ b/Week 1/Lecture Notes/KnapsackExample.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="760" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Example in lecture" sheetId="1" r:id="rId1"/>
     <sheet name="ks_4_0" sheetId="2" r:id="rId2"/>
+    <sheet name="Results" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,8 +20,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Jez</author>
+  </authors>
+  <commentList>
+    <comment ref="C14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+required -Xmx4096</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+required Xmx8192m</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>Maximise</t>
   </si>
@@ -131,13 +190,88 @@
   </si>
   <si>
     <t xml:space="preserve">x4 + x3 </t>
+  </si>
+  <si>
+    <t>[this line states that the combined weight of all selected items must be less than the capacity of 7]</t>
+  </si>
+  <si>
+    <t>[this line states that the objective is to get the highest value based upon the given item values]</t>
+  </si>
+  <si>
+    <t>[this line states that each item must be set as 0 or 1 (to show whether it's been selected)]</t>
+  </si>
+  <si>
+    <t>Algorithm/Data File</t>
+  </si>
+  <si>
+    <t>Table of maximum values</t>
+  </si>
+  <si>
+    <t>DynamicProgrammingKnapsackSolver</t>
+  </si>
+  <si>
+    <t>ks_4_0</t>
+  </si>
+  <si>
+    <t>ks_19_0</t>
+  </si>
+  <si>
+    <t>ks_30_0</t>
+  </si>
+  <si>
+    <t>ks_40_0</t>
+  </si>
+  <si>
+    <t>ks_45_0</t>
+  </si>
+  <si>
+    <t>ks_10000_0</t>
+  </si>
+  <si>
+    <t>ks_100_2</t>
+  </si>
+  <si>
+    <t>ks_300_0</t>
+  </si>
+  <si>
+    <t>ks_50_1</t>
+  </si>
+  <si>
+    <t>ks_1000_0</t>
+  </si>
+  <si>
+    <t>ks_60_0</t>
+  </si>
+  <si>
+    <t>ks_100_0</t>
+  </si>
+  <si>
+    <t>ks_200_0</t>
+  </si>
+  <si>
+    <t>ks_400_0</t>
+  </si>
+  <si>
+    <t>ks_500_0</t>
+  </si>
+  <si>
+    <t>ks_100_1</t>
+  </si>
+  <si>
+    <t>ks_200_1</t>
+  </si>
+  <si>
+    <t>ks_50_0</t>
+  </si>
+  <si>
+    <t>couldn't solve - required heap size over 12288m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,6 +294,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -409,7 +563,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -417,8 +571,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -436,14 +620,48 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -776,14 +994,14 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -791,31 +1009,40 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="60">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" s="17" t="s">
+        <v>38</v>
+      </c>
       <c r="G3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="60">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
+      <c r="C4" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="G4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="60">
       <c r="B5" t="s">
         <v>3</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="G5" t="s">
         <v>18</v>
@@ -1140,7 +1367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A10" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -1544,4 +1771,187 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6">
+        <v>12248</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <v>99798</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8">
+        <v>99924</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9">
+        <v>23974</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <v>142156</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>5345</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12">
+        <v>99837</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13">
+        <v>99837</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14">
+        <v>1333930</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15">
+        <v>10892</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16">
+        <v>100236</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17">
+        <v>1103604</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>1688692</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20">
+        <v>54939</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21">
+        <v>109899</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change KnapsackSolver to interface
</commit_message>
<xml_diff>
--- a/Week 1/Lecture Notes/KnapsackExample.xlsx
+++ b/Week 1/Lecture Notes/KnapsackExample.xlsx
@@ -27,7 +27,7 @@
     <author>Jez</author>
   </authors>
   <commentList>
-    <comment ref="F14" authorId="0">
+    <comment ref="F18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0">
+    <comment ref="F20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -75,12 +75,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="G22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+required -Xss4096m</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
   <si>
     <t>Maximise</t>
   </si>
@@ -278,6 +302,9 @@
   </si>
   <si>
     <t>BranchAndBoundKnapsackSolver</t>
+  </si>
+  <si>
+    <t>FileNumber</t>
   </si>
 </sst>
 </file>
@@ -705,7 +732,17 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2512,10 +2549,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G22"/>
+  <dimension ref="A2:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2526,12 +2563,15 @@
     <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
+    <row r="2" spans="1:7">
       <c r="B2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
       <c r="B4" t="s">
         <v>40</v>
       </c>
@@ -2551,7 +2591,10 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>1</v>
+      </c>
       <c r="B5" t="s">
         <v>43</v>
       </c>
@@ -2572,70 +2615,82 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>7</v>
+      </c>
       <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>5000</v>
+      </c>
+      <c r="E6">
+        <f>C6*D6</f>
+        <v>250000</v>
+      </c>
+      <c r="F6">
+        <v>5345</v>
+      </c>
+      <c r="G6" s="21">
+        <v>5304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>19</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>31181</v>
       </c>
-      <c r="E6">
-        <f t="shared" ref="E6:E22" si="0">C6*D6</f>
+      <c r="E7">
+        <f>C7*D7</f>
         <v>592439</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>12248</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <v>12248</v>
       </c>
     </row>
-    <row r="7" spans="2:7">
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
-      <c r="D7">
-        <v>100000</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>3000000</v>
-      </c>
-      <c r="F7">
-        <v>99798</v>
-      </c>
-      <c r="G7">
-        <v>99798</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8">
-        <v>40</v>
-      </c>
-      <c r="D8">
-        <v>100000</v>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="18">
+        <v>100</v>
+      </c>
+      <c r="D8" s="18">
+        <v>10000</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>4000000</v>
+        <f>C8*D8</f>
+        <v>1000000</v>
       </c>
       <c r="F8">
-        <v>99924</v>
-      </c>
-      <c r="G8">
-        <v>99924</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7">
+        <v>10892</v>
+      </c>
+      <c r="G8" s="21">
+        <v>10851</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>5</v>
+      </c>
       <c r="B9" t="s">
         <v>47</v>
       </c>
@@ -2646,7 +2701,7 @@
         <v>58181</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f>C9*D9</f>
         <v>2618145</v>
       </c>
       <c r="F9">
@@ -2656,49 +2711,58 @@
         <v>23974</v>
       </c>
     </row>
-    <row r="10" spans="2:7">
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>3</v>
+      </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D10">
-        <v>341045</v>
+        <v>100000</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>17052250</v>
+        <f>C10*D10</f>
+        <v>3000000</v>
       </c>
       <c r="F10">
-        <v>142156</v>
-      </c>
-      <c r="G10" s="21">
-        <v>141960</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7">
+        <v>99798</v>
+      </c>
+      <c r="G10">
+        <v>99798</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>4</v>
+      </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D11">
-        <v>5000</v>
+        <v>100000</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>250000</v>
+        <f>C11*D11</f>
+        <v>4000000</v>
       </c>
       <c r="F11">
-        <v>5345</v>
-      </c>
-      <c r="G11" s="21">
-        <v>5304</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7">
+        <v>99924</v>
+      </c>
+      <c r="G11">
+        <v>99924</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>8</v>
+      </c>
       <c r="B12" t="s">
         <v>53</v>
       </c>
@@ -2709,7 +2773,7 @@
         <v>100000</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f>C12*D12</f>
         <v>6000000</v>
       </c>
       <c r="F12">
@@ -2719,7 +2783,10 @@
         <v>99837</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>9</v>
+      </c>
       <c r="B13" t="s">
         <v>54</v>
       </c>
@@ -2730,7 +2797,7 @@
         <v>100000</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f>C13*D13</f>
         <v>10000000</v>
       </c>
       <c r="F13">
@@ -2740,175 +2807,202 @@
         <v>99837</v>
       </c>
     </row>
-    <row r="14" spans="2:7">
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>6</v>
+      </c>
       <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>341045</v>
+      </c>
+      <c r="E14">
+        <f>C14*D14</f>
+        <v>17052250</v>
+      </c>
+      <c r="F14">
+        <v>142156</v>
+      </c>
+      <c r="G14" s="21">
+        <v>141960</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15">
+        <v>200</v>
+      </c>
+      <c r="D15">
+        <v>100000</v>
+      </c>
+      <c r="E15">
+        <f>C15*D15</f>
+        <v>20000000</v>
+      </c>
+      <c r="F15">
+        <v>100236</v>
+      </c>
+      <c r="G15">
+        <v>100236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16">
+        <v>500</v>
+      </c>
+      <c r="D16">
+        <v>50000</v>
+      </c>
+      <c r="E16">
+        <f>C16*D16</f>
+        <v>25000000</v>
+      </c>
+      <c r="F16">
+        <v>54939</v>
+      </c>
+      <c r="G16" s="21">
+        <v>54928</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17">
+        <v>1000</v>
+      </c>
+      <c r="D17">
+        <v>100000</v>
+      </c>
+      <c r="E17">
+        <f>C17*D17</f>
+        <v>100000000</v>
+      </c>
+      <c r="F17">
+        <v>109899</v>
+      </c>
+      <c r="G17" s="21">
+        <v>109894</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
         <v>58</v>
       </c>
-      <c r="C14">
+      <c r="C18">
         <v>100</v>
       </c>
-      <c r="D14">
+      <c r="D18">
         <v>3190802</v>
       </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
+      <c r="E18">
+        <f>C18*D18</f>
         <v>319080200</v>
       </c>
-      <c r="F14">
+      <c r="F18">
         <v>1333930</v>
       </c>
-      <c r="G14">
+      <c r="G18">
         <v>1333930</v>
       </c>
     </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="18">
-        <v>100</v>
-      </c>
-      <c r="D15" s="18">
-        <v>10000</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
-      </c>
-      <c r="F15">
-        <v>10892</v>
-      </c>
-      <c r="G15" s="21">
-        <v>10851</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16">
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19">
         <v>200</v>
       </c>
-      <c r="D16">
-        <v>100000</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>20000000</v>
-      </c>
-      <c r="F16">
-        <v>100236</v>
-      </c>
-      <c r="G16">
-        <v>100236</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17">
-        <v>200</v>
-      </c>
-      <c r="D17">
+      <c r="D19">
         <v>2640230</v>
       </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
+      <c r="E19">
+        <f>C19*D19</f>
         <v>528046000</v>
       </c>
-      <c r="F17">
+      <c r="F19">
         <v>1103604</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G19" s="21">
         <v>1103372</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
-      <c r="B18" t="s">
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
         <v>50</v>
       </c>
-      <c r="C18">
+      <c r="C20">
         <v>300</v>
       </c>
-      <c r="D18">
+      <c r="D20">
         <v>4040184</v>
       </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
+      <c r="E20">
+        <f>C20*D20</f>
         <v>1212055200</v>
       </c>
-      <c r="F18">
+      <c r="F20">
         <v>1688692</v>
       </c>
-      <c r="G18">
+      <c r="G20">
         <v>1688392</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
-      <c r="B19" t="s">
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
         <v>56</v>
       </c>
-      <c r="C19">
+      <c r="C21">
         <v>400</v>
       </c>
-      <c r="D19">
+      <c r="D21">
         <v>9486367</v>
       </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
+      <c r="E21">
+        <f>C21*D21</f>
         <v>3794546800</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F21" t="s">
         <v>61</v>
       </c>
-      <c r="G19">
+      <c r="G21">
         <v>3967168</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
-      <c r="B20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20">
-        <v>500</v>
-      </c>
-      <c r="D20">
-        <v>50000</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>25000000</v>
-      </c>
-      <c r="F20">
-        <v>54939</v>
-      </c>
-      <c r="G20" s="21">
-        <v>54928</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21">
-        <v>1000</v>
-      </c>
-      <c r="D21">
-        <v>100000</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>100000000</v>
-      </c>
-      <c r="F21">
-        <v>109899</v>
-      </c>
-      <c r="G21" s="21">
-        <v>109894</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>18</v>
+      </c>
       <c r="B22" t="s">
         <v>48</v>
       </c>
@@ -2919,16 +3013,22 @@
         <v>1000000</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f>C22*D22</f>
         <v>10000000000</v>
       </c>
       <c r="F22" t="s">
         <v>61</v>
       </c>
+      <c r="G22">
+        <v>1099883</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G5:G21">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <sortState ref="A5:G22">
+    <sortCondition ref="E5:E22"/>
+  </sortState>
+  <conditionalFormatting sqref="G5:G22">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>"&lt;&gt;$F5"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
changed node to use list of item ids instead of item objects
</commit_message>
<xml_diff>
--- a/Week 1/Lecture Notes/KnapsackExample.xlsx
+++ b/Week 1/Lecture Notes/KnapsackExample.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="46140" yWindow="200" windowWidth="28800" windowHeight="16240" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13020" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Example in lecture" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
   <si>
     <t>Maximise</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>FileNumber</t>
+  </si>
+  <si>
+    <t>BranchAndBound_DepthFirst_LinearRegression_KnapsackSolver</t>
   </si>
 </sst>
 </file>
@@ -732,7 +735,157 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1977,7 +2130,7 @@
         <v>40006</v>
       </c>
       <c r="E11" s="19">
-        <f>C11/D11</f>
+        <f t="shared" ref="E11:E29" si="0">C11/D11</f>
         <v>0.41376293555966603</v>
       </c>
     </row>
@@ -1992,7 +2145,7 @@
         <v>32708</v>
       </c>
       <c r="E12" s="19">
-        <f>C12/D12</f>
+        <f t="shared" si="0"/>
         <v>0.41286535404182462</v>
       </c>
     </row>
@@ -2007,7 +2160,7 @@
         <v>9656</v>
       </c>
       <c r="E13" s="19">
-        <f>C13/D13</f>
+        <f t="shared" si="0"/>
         <v>0.40161557580778789</v>
       </c>
       <c r="F13">
@@ -2030,7 +2183,7 @@
         <v>10372</v>
       </c>
       <c r="E14" s="19">
-        <f>C14/D14</f>
+        <f t="shared" si="0"/>
         <v>0.39876590821442343</v>
       </c>
     </row>
@@ -2045,7 +2198,7 @@
         <v>7390</v>
       </c>
       <c r="E15" s="19">
-        <f>C15/D15</f>
+        <f t="shared" si="0"/>
         <v>0.39851150202976998</v>
       </c>
     </row>
@@ -2060,7 +2213,7 @@
         <v>7280</v>
       </c>
       <c r="E16" s="19">
-        <f>C16/D16</f>
+        <f t="shared" si="0"/>
         <v>0.39697802197802196</v>
       </c>
     </row>
@@ -2075,7 +2228,7 @@
         <v>4990</v>
       </c>
       <c r="E17" s="19">
-        <f>C17/D17</f>
+        <f t="shared" si="0"/>
         <v>0.38977955911823647</v>
       </c>
     </row>
@@ -2090,7 +2243,7 @@
         <v>4830</v>
       </c>
       <c r="E18" s="19">
-        <f>C18/D18</f>
+        <f t="shared" si="0"/>
         <v>0.38612836438923398</v>
       </c>
     </row>
@@ -2105,7 +2258,7 @@
         <v>3926</v>
       </c>
       <c r="E19" s="19">
-        <f>C19/D19</f>
+        <f t="shared" si="0"/>
         <v>0.38537952114111057</v>
       </c>
     </row>
@@ -2120,7 +2273,7 @@
         <v>4766</v>
       </c>
       <c r="E20" s="19">
-        <f>C20/D20</f>
+        <f t="shared" si="0"/>
         <v>0.38459924464960132</v>
       </c>
     </row>
@@ -2135,7 +2288,7 @@
         <v>2744</v>
       </c>
       <c r="E21" s="19">
-        <f>C21/D21</f>
+        <f t="shared" si="0"/>
         <v>0.37244897959183676</v>
       </c>
     </row>
@@ -2150,7 +2303,7 @@
         <v>2624</v>
       </c>
       <c r="E22" s="19">
-        <f>C22/D22</f>
+        <f t="shared" si="0"/>
         <v>0.36661585365853661</v>
       </c>
     </row>
@@ -2165,7 +2318,7 @@
         <v>3114</v>
       </c>
       <c r="E23" s="19">
-        <f>C23/D23</f>
+        <f t="shared" si="0"/>
         <v>0.3554913294797688</v>
       </c>
     </row>
@@ -2180,7 +2333,7 @@
         <v>3102</v>
       </c>
       <c r="E24" s="19">
-        <f>C24/D24</f>
+        <f t="shared" si="0"/>
         <v>0.35493230174081236</v>
       </c>
     </row>
@@ -2195,7 +2348,7 @@
         <v>3020</v>
       </c>
       <c r="E25" s="19">
-        <f>C25/D25</f>
+        <f t="shared" si="0"/>
         <v>0.35099337748344372</v>
       </c>
     </row>
@@ -2210,7 +2363,7 @@
         <v>2310</v>
       </c>
       <c r="E26" s="19">
-        <f>C26/D26</f>
+        <f t="shared" si="0"/>
         <v>0.34848484848484851</v>
       </c>
     </row>
@@ -2225,7 +2378,7 @@
         <v>2078</v>
       </c>
       <c r="E27" s="19">
-        <f>C27/D27</f>
+        <f t="shared" si="0"/>
         <v>0.33156881616939365</v>
       </c>
     </row>
@@ -2240,7 +2393,7 @@
         <v>2034</v>
       </c>
       <c r="E28" s="19">
-        <f>C28/D28</f>
+        <f t="shared" si="0"/>
         <v>0.32792527040314651</v>
       </c>
     </row>
@@ -2255,7 +2408,7 @@
         <v>1142</v>
       </c>
       <c r="E29" s="19">
-        <f>C29/D29</f>
+        <f t="shared" si="0"/>
         <v>0.28108581436077057</v>
       </c>
     </row>
@@ -2549,10 +2702,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G22"/>
+  <dimension ref="A2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2561,37 +2714,41 @@
     <col min="3" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="42.33203125" customWidth="1"/>
     <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="B2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" s="17" customFormat="1" ht="30">
+      <c r="A4" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2605,7 +2762,7 @@
         <v>11</v>
       </c>
       <c r="E5">
-        <f>C5*D5</f>
+        <f t="shared" ref="E5:E22" si="0">C5*D5</f>
         <v>44</v>
       </c>
       <c r="F5">
@@ -2614,8 +2771,11 @@
       <c r="G5">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>7</v>
       </c>
@@ -2629,7 +2789,7 @@
         <v>5000</v>
       </c>
       <c r="E6">
-        <f>C6*D6</f>
+        <f t="shared" si="0"/>
         <v>250000</v>
       </c>
       <c r="F6">
@@ -2638,8 +2798,11 @@
       <c r="G6" s="21">
         <v>5304</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>5304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2653,7 +2816,7 @@
         <v>31181</v>
       </c>
       <c r="E7">
-        <f>C7*D7</f>
+        <f t="shared" si="0"/>
         <v>592439</v>
       </c>
       <c r="F7">
@@ -2662,8 +2825,11 @@
       <c r="G7">
         <v>12248</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>12248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>11</v>
       </c>
@@ -2677,7 +2843,7 @@
         <v>10000</v>
       </c>
       <c r="E8">
-        <f>C8*D8</f>
+        <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
       <c r="F8">
@@ -2686,8 +2852,11 @@
       <c r="G8" s="21">
         <v>10851</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <v>10851</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2701,7 +2870,7 @@
         <v>58181</v>
       </c>
       <c r="E9">
-        <f>C9*D9</f>
+        <f t="shared" si="0"/>
         <v>2618145</v>
       </c>
       <c r="F9">
@@ -2710,8 +2879,11 @@
       <c r="G9">
         <v>23974</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9">
+        <v>23974</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>3</v>
       </c>
@@ -2725,7 +2897,7 @@
         <v>100000</v>
       </c>
       <c r="E10">
-        <f>C10*D10</f>
+        <f t="shared" si="0"/>
         <v>3000000</v>
       </c>
       <c r="F10">
@@ -2734,8 +2906,11 @@
       <c r="G10">
         <v>99798</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10">
+        <v>99798</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>4</v>
       </c>
@@ -2749,7 +2924,7 @@
         <v>100000</v>
       </c>
       <c r="E11">
-        <f>C11*D11</f>
+        <f t="shared" si="0"/>
         <v>4000000</v>
       </c>
       <c r="F11">
@@ -2758,8 +2933,11 @@
       <c r="G11">
         <v>99924</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11">
+        <v>99924</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2773,7 +2951,7 @@
         <v>100000</v>
       </c>
       <c r="E12">
-        <f>C12*D12</f>
+        <f t="shared" si="0"/>
         <v>6000000</v>
       </c>
       <c r="F12">
@@ -2782,8 +2960,11 @@
       <c r="G12">
         <v>99837</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12">
+        <v>99837</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2797,7 +2978,7 @@
         <v>100000</v>
       </c>
       <c r="E13">
-        <f>C13*D13</f>
+        <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
       <c r="F13">
@@ -2806,8 +2987,11 @@
       <c r="G13">
         <v>99837</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13">
+        <v>99837</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>6</v>
       </c>
@@ -2821,7 +3005,7 @@
         <v>341045</v>
       </c>
       <c r="E14">
-        <f>C14*D14</f>
+        <f t="shared" si="0"/>
         <v>17052250</v>
       </c>
       <c r="F14">
@@ -2830,8 +3014,11 @@
       <c r="G14" s="21">
         <v>141960</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14">
+        <v>141960</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>12</v>
       </c>
@@ -2845,7 +3032,7 @@
         <v>100000</v>
       </c>
       <c r="E15">
-        <f>C15*D15</f>
+        <f t="shared" si="0"/>
         <v>20000000</v>
       </c>
       <c r="F15">
@@ -2854,8 +3041,11 @@
       <c r="G15">
         <v>100236</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15">
+        <v>100236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>16</v>
       </c>
@@ -2869,7 +3059,7 @@
         <v>50000</v>
       </c>
       <c r="E16">
-        <f>C16*D16</f>
+        <f t="shared" si="0"/>
         <v>25000000</v>
       </c>
       <c r="F16">
@@ -2878,8 +3068,11 @@
       <c r="G16" s="21">
         <v>54928</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16">
+        <v>54928</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>17</v>
       </c>
@@ -2893,7 +3086,7 @@
         <v>100000</v>
       </c>
       <c r="E17">
-        <f>C17*D17</f>
+        <f t="shared" si="0"/>
         <v>100000000</v>
       </c>
       <c r="F17">
@@ -2902,8 +3095,11 @@
       <c r="G17" s="21">
         <v>109894</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17">
+        <v>109894</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>10</v>
       </c>
@@ -2917,7 +3113,7 @@
         <v>3190802</v>
       </c>
       <c r="E18">
-        <f>C18*D18</f>
+        <f t="shared" si="0"/>
         <v>319080200</v>
       </c>
       <c r="F18">
@@ -2926,8 +3122,11 @@
       <c r="G18">
         <v>1333930</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18">
+        <v>1333930</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>13</v>
       </c>
@@ -2941,7 +3140,7 @@
         <v>2640230</v>
       </c>
       <c r="E19">
-        <f>C19*D19</f>
+        <f t="shared" si="0"/>
         <v>528046000</v>
       </c>
       <c r="F19">
@@ -2950,8 +3149,11 @@
       <c r="G19" s="21">
         <v>1103372</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19">
+        <v>1103372</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>14</v>
       </c>
@@ -2965,7 +3167,7 @@
         <v>4040184</v>
       </c>
       <c r="E20">
-        <f>C20*D20</f>
+        <f t="shared" si="0"/>
         <v>1212055200</v>
       </c>
       <c r="F20">
@@ -2974,8 +3176,11 @@
       <c r="G20">
         <v>1688392</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20">
+        <v>1688392</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>15</v>
       </c>
@@ -2989,7 +3194,7 @@
         <v>9486367</v>
       </c>
       <c r="E21">
-        <f>C21*D21</f>
+        <f t="shared" si="0"/>
         <v>3794546800</v>
       </c>
       <c r="F21" t="s">
@@ -2998,8 +3203,11 @@
       <c r="G21">
         <v>3967168</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21">
+        <v>3967168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>18</v>
       </c>
@@ -3013,13 +3221,16 @@
         <v>1000000</v>
       </c>
       <c r="E22">
-        <f>C22*D22</f>
+        <f t="shared" si="0"/>
         <v>10000000000</v>
       </c>
       <c r="F22" t="s">
         <v>61</v>
       </c>
       <c r="G22">
+        <v>1099883</v>
+      </c>
+      <c r="H22">
         <v>1099883</v>
       </c>
     </row>
@@ -3027,8 +3238,8 @@
   <sortState ref="A5:G22">
     <sortCondition ref="E5:E22"/>
   </sortState>
-  <conditionalFormatting sqref="G5:G22">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="G5:G22 H5 H7:H22">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>"&lt;&gt;$F5"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>